<commit_message>
insertion finale du totale de participant
</commit_message>
<xml_diff>
--- a/reponses.xlsx
+++ b/reponses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Présence</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total Participants</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +471,9 @@
           <t>Non</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -479,6 +487,40 @@
         </is>
       </c>
       <c r="C3" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bitton</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cohen</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Yair</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>Oui</t>
         </is>

</xml_diff>

<commit_message>
arrangement de la page
</commit_message>
<xml_diff>
--- a/reponses.xlsx
+++ b/reponses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
@@ -578,6 +578,206 @@
       </c>
       <c r="E7" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Edery</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bitton</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bitton</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Bitton</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Bitton</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Bitton</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Bitton</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Edery</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>yaire</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>malik</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>jojo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>